<commit_message>
GeoAODV angle expansion parameterization (angle_expand)
</commit_message>
<xml_diff>
--- a/data/ALLDATA.xlsx
+++ b/data/ALLDATA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AODVFallbacks_SUM_LARP" sheetId="4" r:id="rId1"/>
@@ -481,25 +481,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="135444736"/>
-        <c:axId val="135458816"/>
+        <c:axId val="47112192"/>
+        <c:axId val="47113728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135444736"/>
+        <c:axId val="47112192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135458816"/>
+        <c:crossAx val="47113728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135458816"/>
+        <c:axId val="47113728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,7 +507,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135444736"/>
+        <c:crossAx val="47112192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -520,7 +520,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -949,25 +949,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="136495872"/>
-        <c:axId val="136497408"/>
+        <c:axId val="47934464"/>
+        <c:axId val="47940352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136495872"/>
+        <c:axId val="47934464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136497408"/>
+        <c:crossAx val="47940352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136497408"/>
+        <c:axId val="47940352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,7 +975,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136495872"/>
+        <c:crossAx val="47934464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -988,7 +988,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1417,25 +1417,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="136660864"/>
-        <c:axId val="136662400"/>
+        <c:axId val="47861760"/>
+        <c:axId val="47863296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136660864"/>
+        <c:axId val="47861760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136662400"/>
+        <c:crossAx val="47863296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136662400"/>
+        <c:axId val="47863296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,19 +1443,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136660864"/>
+        <c:crossAx val="47861760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1884,25 +1885,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="136748032"/>
-        <c:axId val="136819456"/>
+        <c:axId val="47903872"/>
+        <c:axId val="47905408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136748032"/>
+        <c:axId val="47903872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136819456"/>
+        <c:crossAx val="47905408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136819456"/>
+        <c:axId val="47905408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1910,19 +1911,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136748032"/>
+        <c:crossAx val="47903872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2351,45 +2353,48 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="146376576"/>
-        <c:axId val="146378112"/>
+        <c:axId val="48027520"/>
+        <c:axId val="48029056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146376576"/>
+        <c:axId val="48027520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146378112"/>
+        <c:crossAx val="48029056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146378112"/>
+        <c:axId val="48029056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.11"/>
+          <c:min val="4.0000000000000008E-2"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146376576"/>
+        <c:crossAx val="48027520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2818,45 +2823,48 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="149584896"/>
-        <c:axId val="149603072"/>
+        <c:axId val="48089728"/>
+        <c:axId val="48099712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="149584896"/>
+        <c:axId val="48089728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149603072"/>
+        <c:crossAx val="48099712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149603072"/>
+        <c:axId val="48099712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.11"/>
+          <c:min val="4.0000000000000008E-2"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149584896"/>
+        <c:crossAx val="48089728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3285,25 +3293,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="149651840"/>
-        <c:axId val="149653376"/>
+        <c:axId val="48147840"/>
+        <c:axId val="48161920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="149651840"/>
+        <c:axId val="48147840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149653376"/>
+        <c:crossAx val="48161920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149653376"/>
+        <c:axId val="48161920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3311,7 +3319,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149651840"/>
+        <c:crossAx val="48147840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3324,7 +3332,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3753,25 +3761,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="149714432"/>
-        <c:axId val="149715968"/>
+        <c:axId val="48214400"/>
+        <c:axId val="48215936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="149714432"/>
+        <c:axId val="48214400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149715968"/>
+        <c:crossAx val="48215936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149715968"/>
+        <c:axId val="48215936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3779,7 +3787,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149714432"/>
+        <c:crossAx val="48214400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3792,7 +3800,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4221,33 +4229,35 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="149781120"/>
-        <c:axId val="149795200"/>
+        <c:axId val="48309376"/>
+        <c:axId val="48310912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="149781120"/>
+        <c:axId val="48309376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149795200"/>
+        <c:crossAx val="48310912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149795200"/>
+        <c:axId val="48310912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.16"/>
+          <c:min val="0.1"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149781120"/>
+        <c:crossAx val="48309376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4260,7 +4270,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4689,25 +4699,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="149876736"/>
-        <c:axId val="149878272"/>
+        <c:axId val="48351488"/>
+        <c:axId val="48361472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="149876736"/>
+        <c:axId val="48351488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149878272"/>
+        <c:crossAx val="48361472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149878272"/>
+        <c:axId val="48361472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4715,7 +4725,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149876736"/>
+        <c:crossAx val="48351488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4728,7 +4738,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5157,25 +5167,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="144212352"/>
-        <c:axId val="144213888"/>
+        <c:axId val="48520192"/>
+        <c:axId val="48546560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144212352"/>
+        <c:axId val="48520192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144213888"/>
+        <c:crossAx val="48546560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144213888"/>
+        <c:axId val="48546560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3000"/>
@@ -5184,20 +5194,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144212352"/>
+        <c:crossAx val="48520192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5626,25 +5635,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="135589248"/>
-        <c:axId val="135599232"/>
+        <c:axId val="47153536"/>
+        <c:axId val="47155072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135589248"/>
+        <c:axId val="47153536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135599232"/>
+        <c:crossAx val="47155072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135599232"/>
+        <c:axId val="47155072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5652,7 +5661,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135589248"/>
+        <c:crossAx val="47153536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5665,7 +5674,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6094,25 +6103,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="144270848"/>
-        <c:axId val="144272384"/>
+        <c:axId val="49639424"/>
+        <c:axId val="49640960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144270848"/>
+        <c:axId val="49639424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144272384"/>
+        <c:crossAx val="49640960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144272384"/>
+        <c:axId val="49640960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3000"/>
@@ -6121,20 +6130,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144270848"/>
+        <c:crossAx val="49639424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6563,25 +6571,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="145795712"/>
-        <c:axId val="145985920"/>
+        <c:axId val="49693440"/>
+        <c:axId val="49694976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145795712"/>
+        <c:axId val="49693440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145985920"/>
+        <c:crossAx val="49694976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145985920"/>
+        <c:axId val="49694976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6589,20 +6597,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145795712"/>
+        <c:crossAx val="49693440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7031,25 +7038,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="146108416"/>
-        <c:axId val="146109952"/>
+        <c:axId val="49731072"/>
+        <c:axId val="49732608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146108416"/>
+        <c:axId val="49731072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146109952"/>
+        <c:crossAx val="49732608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146109952"/>
+        <c:axId val="49732608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7057,20 +7064,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146108416"/>
+        <c:crossAx val="49731072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7499,25 +7505,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="146220160"/>
-        <c:axId val="146221696"/>
+        <c:axId val="48466176"/>
+        <c:axId val="48484352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146220160"/>
+        <c:axId val="48466176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146221696"/>
+        <c:crossAx val="48484352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146221696"/>
+        <c:axId val="48484352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10000"/>
@@ -7526,7 +7532,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146220160"/>
+        <c:crossAx val="48466176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7538,7 +7544,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7967,25 +7973,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="149842176"/>
-        <c:axId val="150704128"/>
+        <c:axId val="49831296"/>
+        <c:axId val="49845376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="149842176"/>
+        <c:axId val="49831296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150704128"/>
+        <c:crossAx val="49845376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150704128"/>
+        <c:axId val="49845376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10000"/>
@@ -7994,7 +8000,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149842176"/>
+        <c:crossAx val="49831296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8006,7 +8012,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8435,25 +8441,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="135652096"/>
-        <c:axId val="135653632"/>
+        <c:axId val="47211648"/>
+        <c:axId val="47213184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135652096"/>
+        <c:axId val="47211648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135653632"/>
+        <c:crossAx val="47213184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135653632"/>
+        <c:axId val="47213184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8461,7 +8467,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135652096"/>
+        <c:crossAx val="47211648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8474,7 +8480,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8903,25 +8909,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="135714688"/>
-        <c:axId val="135716224"/>
+        <c:axId val="47269760"/>
+        <c:axId val="47271296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135714688"/>
+        <c:axId val="47269760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135716224"/>
+        <c:crossAx val="47271296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135716224"/>
+        <c:axId val="47271296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8929,7 +8935,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135714688"/>
+        <c:crossAx val="47269760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8942,7 +8948,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9371,25 +9377,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="135769088"/>
-        <c:axId val="135787264"/>
+        <c:axId val="47303296"/>
+        <c:axId val="47313280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135769088"/>
+        <c:axId val="47303296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135787264"/>
+        <c:crossAx val="47313280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135787264"/>
+        <c:axId val="47313280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9397,19 +9403,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135769088"/>
+        <c:crossAx val="47303296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9838,25 +9845,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="135840128"/>
-        <c:axId val="135841664"/>
+        <c:axId val="47357952"/>
+        <c:axId val="47359488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135840128"/>
+        <c:axId val="47357952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135841664"/>
+        <c:crossAx val="47359488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135841664"/>
+        <c:axId val="47359488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9864,19 +9871,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135840128"/>
+        <c:crossAx val="47357952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10305,25 +10313,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="136152192"/>
-        <c:axId val="136153728"/>
+        <c:axId val="47452928"/>
+        <c:axId val="47454464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136152192"/>
+        <c:axId val="47452928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136153728"/>
+        <c:crossAx val="47454464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136153728"/>
+        <c:axId val="47454464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10331,7 +10339,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136152192"/>
+        <c:crossAx val="47452928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10344,7 +10352,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10773,25 +10781,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="136210688"/>
-        <c:axId val="136237056"/>
+        <c:axId val="47506944"/>
+        <c:axId val="47508480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136210688"/>
+        <c:axId val="47506944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136237056"/>
+        <c:crossAx val="47508480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136237056"/>
+        <c:axId val="47508480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10799,7 +10807,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136210688"/>
+        <c:crossAx val="47506944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10812,7 +10820,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11241,25 +11249,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="136347008"/>
-        <c:axId val="136356992"/>
+        <c:axId val="47544576"/>
+        <c:axId val="47558656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136347008"/>
+        <c:axId val="47544576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136356992"/>
+        <c:crossAx val="47558656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136356992"/>
+        <c:axId val="47558656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11267,7 +11275,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136347008"/>
+        <c:crossAx val="47544576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11280,7 +11288,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -12313,7 +12321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -13133,7 +13141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
@@ -13953,8 +13961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ48"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="Z44" sqref="Z44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>